<commit_message>
mas filtros y reglas de correos y minusuculas
minusuclas
</commit_message>
<xml_diff>
--- a/correos.xlsx
+++ b/correos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\excelAJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\excelToJsEmails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56929B6-9A06-4677-84A5-D60AC5132132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60133F2-8ADB-4B9E-BC8F-7B8C8094F0BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="3075" windowWidth="22680" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Emails" sheetId="1" r:id="rId1"/>
@@ -26,17 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
-  <si>
-    <t>alexander.kristensen@example.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>logan.nicolas@example.com</t>
   </si>
   <si>
-    <t>annabelle.harris@example.com</t>
-  </si>
-  <si>
     <t>manja.klar@example.com</t>
   </si>
   <si>
@@ -61,18 +55,6 @@
     <t>noham.gonzalez@example.com</t>
   </si>
   <si>
-    <t>jesus.dominguez@example.com</t>
-  </si>
-  <si>
-    <t>avery.gagne@example.com</t>
-  </si>
-  <si>
-    <t>belen.guerrero@example.com</t>
-  </si>
-  <si>
-    <t>aylyn.mwswy@example.com</t>
-  </si>
-  <si>
     <t>camille.addy@example.com</t>
   </si>
   <si>
@@ -152,9 +134,6 @@
   </si>
   <si>
     <t>bonnie.pena@example.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">te explicare mas detalladamente y espero se me pueda entender, los datos amarillos son los valores de entrada, lo que necesito es extraer el nombre de la persona o dueño del correo. Entonces por ejemplo tenemos a csuazo@biobiochile.cl --- entonces el nombre seria csuazo. el nombre puede estar antes o despues del arroba. "@". </t>
   </si>
   <si>
     <t>Tengo varias condicion la primera es eliminar los numeros del nombre y 
@@ -179,6 +158,24 @@
   </si>
   <si>
     <t>ventas@example.com</t>
+  </si>
+  <si>
+    <t>CONTACTO@example.com</t>
+  </si>
+  <si>
+    <t>cONTACTO@example.com</t>
+  </si>
+  <si>
+    <t>Contacto@example.com</t>
+  </si>
+  <si>
+    <t>alexander.krist@example.com</t>
+  </si>
+  <si>
+    <t>ServiciO@eCorp.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">te explicare mas detalladamente y espero se me pueda entender, los datos amarillos son los valores de entrada, lo que necesito es extraer el nombre de la persona o dueño del correo. Entonces por ejemplo tenemos a csuazo@biobiochile.cl --- entonces el nombre seria csuazo. el nombre puede estar antes o despues del arroba. "@". </t>
   </si>
 </sst>
 </file>
@@ -595,268 +592,269 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="39" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
+      <c r="A5" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2" t="s">
-        <v>9</v>
+      <c r="A14" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="2" t="s">
-        <v>10</v>
+      <c r="A15" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="2" t="s">
-        <v>11</v>
+      <c r="A17" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="2" t="s">
-        <v>12</v>
+      <c r="A18" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="2" t="s">
-        <v>13</v>
+      <c r="A19" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="2" t="s">
-        <v>14</v>
+      <c r="A20" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -871,8 +869,16 @@
     <hyperlink ref="A26" r:id="rId8" xr:uid="{B3867103-4B5E-45AC-8AEE-98B9058466DB}"/>
     <hyperlink ref="A13" r:id="rId9" xr:uid="{7383F04B-BF6D-413E-8570-E98F22A8E911}"/>
     <hyperlink ref="A16" r:id="rId10" xr:uid="{D472A330-A146-4A47-A7C3-0D3EDA8448AF}"/>
+    <hyperlink ref="A17" r:id="rId11" xr:uid="{0DBD5D46-689F-4106-AEB8-813DB820FAA5}"/>
+    <hyperlink ref="A18" r:id="rId12" xr:uid="{809F4630-820D-4212-BFEF-2B4C3F362E0B}"/>
+    <hyperlink ref="A19" r:id="rId13" xr:uid="{6D054A6C-C009-4F2B-803A-A405EF43D66F}"/>
+    <hyperlink ref="A20" r:id="rId14" xr:uid="{A2D83E7F-F3C3-48F1-9F2C-3B5D4FAFBD0C}"/>
+    <hyperlink ref="A15" r:id="rId15" xr:uid="{97781142-03DF-4026-AAE6-B3FC146BACC7}"/>
+    <hyperlink ref="A14" r:id="rId16" xr:uid="{E427B47F-E1E6-49CC-80A2-0F086F0487C5}"/>
+    <hyperlink ref="A5" r:id="rId17" xr:uid="{9F66EA43-9B3E-4A15-8BB8-DC9708B8AAD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -880,15 +886,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E05879F-D137-4FFA-BE73-3FD14D293798}">
   <dimension ref="E5:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="5" spans="5:18">
       <c r="E5" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -922,7 +928,7 @@
     </row>
     <row r="7" spans="5:18">
       <c r="E7" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>

</xml_diff>